<commit_message>
Added Home Assignment 2
</commit_message>
<xml_diff>
--- a/QAtraining/HomeAssignment2/Yahoo Registeration Test Script (Autosaved).xlsx
+++ b/QAtraining/HomeAssignment2/Yahoo Registeration Test Script (Autosaved).xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vrindha\Desktop\QA training\Assignment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="7590" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="7600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mail Id Creation" sheetId="3" r:id="rId1"/>
     <sheet name="Test Case" sheetId="1" r:id="rId2"/>
     <sheet name="Test Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -112,9 +110,6 @@
     <t>User enters "123"</t>
   </si>
   <si>
-    <t>Warning Message "Numbers and special characters are not allowed"</t>
-  </si>
-  <si>
     <t>User enters First Name "123"</t>
   </si>
   <si>
@@ -145,27 +140,12 @@
     <t>Positive Max</t>
   </si>
   <si>
-    <t>User enters First Name all alpha=1 char</t>
-  </si>
-  <si>
-    <t>User enters First Name all alpha=0 char</t>
-  </si>
-  <si>
-    <t>User enters First Name all alpha=40 char</t>
-  </si>
-  <si>
-    <t>User enters First Name all alpha=41 char</t>
-  </si>
-  <si>
     <t>User is prompted with message First Name is required</t>
   </si>
   <si>
     <t>Negative max</t>
   </si>
   <si>
-    <t>User is not allowed to enter more than 40 alphabetic char</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -184,18 +164,6 @@
     <t>User enters Last Name "ABI"</t>
   </si>
   <si>
-    <t>User enters Last Name all alpha=1 char</t>
-  </si>
-  <si>
-    <t>User enters Last Name all alpha=0 char</t>
-  </si>
-  <si>
-    <t>User enters Last Name all alpha=40 char</t>
-  </si>
-  <si>
-    <t>User enters Last Name all alpha=41 char</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -298,9 +266,6 @@
     <t>User enters "Abish"</t>
   </si>
   <si>
-    <t>Username enters a combination of alpha underscore and period=4 char</t>
-  </si>
-  <si>
     <t>User can create First name successfully</t>
   </si>
   <si>
@@ -313,18 +278,6 @@
     <t>Username is allowed to create a username depending on the availability of the same in the database without allowing duplicate entries</t>
   </si>
   <si>
-    <t>Username enters a combination of alpha underscore and period =3 char</t>
-  </si>
-  <si>
-    <t>Username enters a combination of alpha underscore and period =32 char</t>
-  </si>
-  <si>
-    <t>Username enters a combination of alpha underscore and period =33 char</t>
-  </si>
-  <si>
-    <t>Validation Message "Your username must be at least 4 characters long"</t>
-  </si>
-  <si>
     <t>User leaves the password field blank</t>
   </si>
   <si>
@@ -355,18 +308,6 @@
     <t>Password is created in encrypted form</t>
   </si>
   <si>
-    <t>Username enters a combination of alpha numeric and special char =3 char</t>
-  </si>
-  <si>
-    <t>Username enters a combination of alpha numeric and special char =33 char</t>
-  </si>
-  <si>
-    <t>Username enters a combination of alpha numeric and special char =32char</t>
-  </si>
-  <si>
-    <t>Username enters a combination of alpha numeric and special char =4 char</t>
-  </si>
-  <si>
     <t>A message is displayed "This is not a valid mobile number"</t>
   </si>
   <si>
@@ -374,15 +315,6 @@
   </si>
   <si>
     <t>Mobile number is created</t>
-  </si>
-  <si>
-    <t>Username enters numeric combo =10 char</t>
-  </si>
-  <si>
-    <t>Username enters numeric combo =9 char</t>
-  </si>
-  <si>
-    <t>Username enters numeric combo =11 char</t>
   </si>
   <si>
     <t>User is not allowed to enter more than 10 number combo</t>
@@ -865,11 +797,77 @@
   <si>
     <t>fdfdf</t>
   </si>
+  <si>
+    <t>Warning Message "Numbers and special Characteracters are not allowed"</t>
+  </si>
+  <si>
+    <t>User enters First Name all alpha=1 Character</t>
+  </si>
+  <si>
+    <t>User enters First Name all alpha=0 Character</t>
+  </si>
+  <si>
+    <t>User enters First Name all alpha=40 Character</t>
+  </si>
+  <si>
+    <t>User enters First Name all alpha=41 Character</t>
+  </si>
+  <si>
+    <t>User is not allowed to enter more than 40 alphabetic Character</t>
+  </si>
+  <si>
+    <t>User enters Last Name all alpha=1 Character</t>
+  </si>
+  <si>
+    <t>User enters Last Name all alpha=0 Character</t>
+  </si>
+  <si>
+    <t>User enters Last Name all alpha=40 Character</t>
+  </si>
+  <si>
+    <t>User enters Last Name all alpha=41 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha underscore and period=4 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha underscore and period =3 Character</t>
+  </si>
+  <si>
+    <t>Validation Message "Your username must be at least 4 Characteracters long"</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha underscore and period =32 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha underscore and period =33 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha numeric and special Character =4 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha numeric and special Character =3 Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha numeric and special Character =32Character</t>
+  </si>
+  <si>
+    <t>Username enters a combination of alpha numeric and special Character =33 Character</t>
+  </si>
+  <si>
+    <t>Username enters numeric combo =10 Character</t>
+  </si>
+  <si>
+    <t>Username enters numeric combo =9 Character</t>
+  </si>
+  <si>
+    <t>Username enters numeric combo =11 Character</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -974,11 +972,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -987,7 +985,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -995,17 +993,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1015,7 +1013,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1023,12 +1021,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1037,18 +1035,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1167,7 +1165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1202,7 +1200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1379,7 +1377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1393,20 +1391,20 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15" thickBot="1"/>
+    <row r="4" spans="2:15">
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -1422,7 +1420,7 @@
       <c r="N4" s="13"/>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" s="15"/>
       <c r="C5" s="21"/>
       <c r="D5" s="22" t="s">
@@ -1440,7 +1438,7 @@
       <c r="N5" s="16"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
@@ -1456,7 +1454,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -1466,13 +1464,13 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
@@ -1480,23 +1478,23 @@
       <c r="N7" s="16"/>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
@@ -1504,23 +1502,23 @@
       <c r="N8" s="16"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" s="15"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
@@ -1528,23 +1526,23 @@
       <c r="N9" s="16"/>
       <c r="O9" s="17"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
@@ -1552,23 +1550,23 @@
       <c r="N10" s="16"/>
       <c r="O10" s="17"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
@@ -1576,77 +1574,77 @@
       <c r="N11" s="16"/>
       <c r="O11" s="17"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="17"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="23" t="s">
         <v>65</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>75</v>
       </c>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="O13" s="17"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
@@ -1654,23 +1652,23 @@
       <c r="N14" s="16"/>
       <c r="O14" s="17"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
@@ -1678,7 +1676,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="17"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1694,19 +1692,19 @@
       <c r="N16" s="16"/>
       <c r="O16" s="17"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
       <c r="J17" s="23" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
@@ -1714,7 +1712,7 @@
       <c r="N17" s="16"/>
       <c r="O17" s="17"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -1730,7 +1728,7 @@
       <c r="N18" s="16"/>
       <c r="O18" s="17"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -1746,11 +1744,11 @@
       <c r="N19" s="16"/>
       <c r="O19" s="17"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20" s="15"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="16"/>
@@ -1764,7 +1762,7 @@
       <c r="N20" s="16"/>
       <c r="O20" s="17"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15">
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1780,23 +1778,23 @@
       <c r="N21" s="16"/>
       <c r="O21" s="17"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
@@ -1804,23 +1802,23 @@
       <c r="N22" s="16"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15">
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
@@ -1828,7 +1826,7 @@
       <c r="N23" s="16"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15">
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -1844,19 +1842,19 @@
       <c r="N24" s="16"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15">
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="J25" s="23" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
@@ -1864,7 +1862,7 @@
       <c r="N25" s="16"/>
       <c r="O25" s="17"/>
     </row>
-    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" ht="15" thickBot="1">
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -1882,29 +1880,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AD115"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="8" t="s">
@@ -1938,7 +1941,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1948,7 +1951,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1958,7 +1961,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1968,7 +1971,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1993,7 +1996,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -2006,7 +2009,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="11">
         <v>1.1000000000000001</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="B12" s="10" t="s">
         <v>23</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="28">
       <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="28">
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
@@ -2050,13 +2053,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28">
       <c r="A18">
         <v>1.2</v>
       </c>
@@ -2064,714 +2067,714 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28">
+      <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="E20" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="E21" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42">
+      <c r="C22" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="E22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="4" t="s">
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C23" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28">
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28">
       <c r="A28">
         <v>1.3</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28">
       <c r="C29" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28">
       <c r="C30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28">
       <c r="C31" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="42">
       <c r="C32" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:5">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="C33" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28">
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="C34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="28">
       <c r="B36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>55</v>
+        <v>174</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>1.4</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="42">
       <c r="B38" s="25"/>
       <c r="C38" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="42">
       <c r="B39" s="25"/>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="28">
       <c r="B40" s="25"/>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28">
       <c r="B41" s="25"/>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="42">
       <c r="B42" s="25"/>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="28">
       <c r="C43" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="56">
       <c r="C44" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="56">
       <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28">
+      <c r="B46" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="C46" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="56">
+      <c r="B47" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>38</v>
-      </c>
       <c r="C47" s="4" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28">
       <c r="B48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>1.5</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28">
       <c r="C51" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="42">
       <c r="C52" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="42">
       <c r="C53" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="42">
       <c r="C54" s="4" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="42">
       <c r="C55" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="C56" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="28">
       <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="42">
+      <c r="B58" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="C58" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="28">
+      <c r="B59" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>38</v>
-      </c>
       <c r="C59" s="4" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="42">
       <c r="B60" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>1.6</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="28">
       <c r="C62" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="28">
       <c r="C63" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="C64" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="B65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28">
+      <c r="B66" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="C66" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="B67" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>38</v>
-      </c>
       <c r="C67" s="4" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28">
       <c r="B68" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>1.7</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="C70" s="4" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="C71" s="4" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="C72" s="4" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="28">
       <c r="C73" s="4" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>1.8</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28">
       <c r="B75" s="9"/>
       <c r="C75" s="4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="C76" s="4" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="C77" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>1.9</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="28">
       <c r="C80" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>1.1000000000000001</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="28">
       <c r="C82" s="4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="E82" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>1.1100000000000001</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="98">
       <c r="C84" s="4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="28">
       <c r="C85" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="B86" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="28">
       <c r="C87" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="28">
       <c r="C88" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="C89" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="B90" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="28">
+      <c r="B91" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="C91" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="B92" t="s">
         <v>37</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>38</v>
-      </c>
       <c r="C92" s="4" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="28">
       <c r="B93" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C93" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="56">
+      <c r="B95" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B95" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="E95" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="28">
       <c r="B96" s="10" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="70">
       <c r="C97" s="4" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="11"/>
       <c r="B99" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="B101" s="10" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
@@ -2783,7 +2786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="28">
       <c r="C102" s="4" t="s">
         <v>19</v>
       </c>
@@ -2794,84 +2797,89 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6">
       <c r="C103" s="4"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="56">
       <c r="C104" s="4" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="56">
       <c r="C105" s="4" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="56">
       <c r="C106" s="4" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="56">
       <c r="C107" s="4" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="56">
       <c r="C108" s="4" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="28">
       <c r="C109" s="4" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="42">
       <c r="C110" s="4" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6">
       <c r="C114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:6">
       <c r="C115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2879,61 +2887,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="36" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="C4" s="36"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15" thickBot="1"/>
+    <row r="6" spans="2:11" ht="28">
       <c r="B6" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="K6" s="29"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -2945,18 +2953,18 @@
       <c r="J7" s="31"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="30" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="F8" s="31">
         <v>1321433435</v>
@@ -2965,63 +2973,63 @@
         <v>36863</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="I8" s="31"/>
       <c r="J8" s="31"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="30"/>
       <c r="C9" s="31" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="G9" s="38">
         <v>35403</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="30" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="G10" s="38">
         <v>29314</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="30"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -3033,7 +3041,7 @@
       <c r="J11" s="31"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
@@ -3045,7 +3053,7 @@
       <c r="J12" s="31"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="30"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -3057,7 +3065,7 @@
       <c r="J13" s="31"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -3069,7 +3077,7 @@
       <c r="J14" s="31"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -3081,7 +3089,7 @@
       <c r="J15" s="31"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="30"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -3093,7 +3101,7 @@
       <c r="J16" s="31"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" thickBot="1">
       <c r="B17" s="33"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
@@ -3105,25 +3113,25 @@
       <c r="J17" s="34"/>
       <c r="K17" s="35"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="36" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="15" thickBot="1"/>
+    <row r="21" spans="2:11">
       <c r="B21" s="41" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="39"/>
       <c r="F21" s="39"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11">
       <c r="B22" s="30"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
@@ -3131,19 +3139,19 @@
       <c r="F22" s="31"/>
       <c r="G22" s="32"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11">
       <c r="B23" s="30"/>
       <c r="C23" s="31" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="32"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="30" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -3151,43 +3159,43 @@
       <c r="F24" s="31"/>
       <c r="G24" s="32"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11">
       <c r="B25" s="30" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="32"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11">
       <c r="B26" s="30" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="32"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11">
       <c r="B27" s="30" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
       <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11">
       <c r="B28" s="30"/>
       <c r="C28" s="31"/>
       <c r="D28" s="31"/>
@@ -3195,7 +3203,7 @@
       <c r="F28" s="31"/>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="15" thickBot="1">
       <c r="B29" s="33"/>
       <c r="C29" s="34"/>
       <c r="D29" s="34"/>
@@ -3205,5 +3213,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>